<commit_message>
reporting, highlighting and screenshots added
</commit_message>
<xml_diff>
--- a/reports/protractorresults.xlsx
+++ b/reports/protractorresults.xlsx
@@ -267,7 +267,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>3.159</v>
+        <v>2.232</v>
       </c>
     </row>
     <row r="3" spans="3:3">
@@ -284,7 +284,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>1.597</v>
+        <v>1.483</v>
       </c>
     </row>
     <row r="4" spans="4:4">
@@ -301,7 +301,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>1.86</v>
+        <v>1.389</v>
       </c>
     </row>
     <row r="5" spans="5:5">
@@ -318,7 +318,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>1.126</v>
+        <v>1.698</v>
       </c>
     </row>
     <row r="6" spans="6:6">
@@ -335,7 +335,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>4.863</v>
+        <v>7.462</v>
       </c>
     </row>
   </sheetData>
@@ -392,7 +392,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>3.159</v>
+        <v>2.232</v>
       </c>
     </row>
     <row r="3" spans="3:3">
@@ -409,7 +409,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>1.597</v>
+        <v>1.483</v>
       </c>
     </row>
     <row r="4" spans="4:4">
@@ -426,7 +426,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>1.86</v>
+        <v>1.389</v>
       </c>
     </row>
     <row r="5" spans="5:5">
@@ -443,7 +443,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>1.126</v>
+        <v>1.698</v>
       </c>
     </row>
     <row r="6" spans="6:6">
@@ -460,7 +460,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>4.863</v>
+        <v>7.462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>